<commit_message>
example run files that were generated
</commit_message>
<xml_diff>
--- a/storage/runs/example-run/workingDir/Analysis/00_LogFile/DataSheet.xlsx
+++ b/storage/runs/example-run/workingDir/Analysis/00_LogFile/DataSheet.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Control</t>
   </si>
@@ -44,18 +41,6 @@
     <t>TREATMENT</t>
   </si>
   <si>
-    <t>Tox-A_R1_98_S2_L008_R1_001_x.fastq.gz</t>
-  </si>
-  <si>
-    <t>Tox-A_R2_S2_L005_R1_001_x.fastq.gz</t>
-  </si>
-  <si>
-    <t>Tox-B_R1_98_S4_L008_R1_001_x.fastq.gz</t>
-  </si>
-  <si>
-    <t>Tox-B_R2_S4_L005_R1_001_x.fastq.gz</t>
-  </si>
-  <si>
     <t>ToxA</t>
   </si>
   <si>
@@ -65,13 +50,10 @@
     <t>ToxA_2</t>
   </si>
   <si>
-    <t>ToxB</t>
-  </si>
-  <si>
-    <t>ToxB_1</t>
-  </si>
-  <si>
-    <t>ToxB_2</t>
+    <t>ToxA_R1_98_S2_L008_R1_001_x.fastq.gz</t>
+  </si>
+  <si>
+    <t>ToxA_R2_S2_L005_R1_001_x.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -432,7 +414,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,91 +430,69 @@
   <sheetData>
     <row spans="1:4" r="1">
       <c s="1" t="s" r="B1">
+        <v>5</v>
+      </c>
+      <c s="1" t="s" r="C1">
+        <v>7</v>
+      </c>
+      <c s="1" t="s" r="D1">
         <v>6</v>
-      </c>
-      <c s="1" t="s" r="C1">
-        <v>8</v>
-      </c>
-      <c s="1" t="s" r="D1">
-        <v>7</v>
       </c>
     </row>
     <row spans="1:4" r="2">
       <c s="1" t="n" r="A2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c t="s" r="B2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c t="s" r="C2">
+        <v>0</v>
+      </c>
+      <c t="s" r="D2">
         <v>1</v>
-      </c>
-      <c t="s" r="D2">
-        <v>2</v>
       </c>
     </row>
     <row spans="1:4" r="3">
       <c s="1" t="n" r="A3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c t="s" r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c t="s" r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row spans="1:4" r="4">
       <c s="1" t="n" r="A4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c t="s" r="B4">
+        <v>11</v>
+      </c>
+      <c t="s" r="C4">
+        <v>8</v>
+      </c>
+      <c t="s" r="D4">
         <v>9</v>
-      </c>
-      <c t="s" r="C4">
-        <v>13</v>
-      </c>
-      <c t="s" r="D4">
-        <v>14</v>
       </c>
     </row>
     <row spans="1:4" r="5">
-      <c s="1" t="s" r="A5"/>
+      <c s="1" t="n" r="A5">
+        <v>3</v>
+      </c>
       <c t="s" r="B5">
+        <v>12</v>
+      </c>
+      <c t="s" r="C5">
+        <v>8</v>
+      </c>
+      <c t="s" r="D5">
         <v>10</v>
-      </c>
-      <c t="s" r="C5">
-        <v>13</v>
-      </c>
-      <c t="s" r="D5">
-        <v>15</v>
-      </c>
-    </row>
-    <row spans="1:4" r="6">
-      <c s="1" t="s" r="A6"/>
-      <c t="s" r="B6">
-        <v>11</v>
-      </c>
-      <c t="s" r="C6">
-        <v>16</v>
-      </c>
-      <c t="s" r="D6">
-        <v>17</v>
-      </c>
-    </row>
-    <row spans="1:4" r="7">
-      <c s="1" t="s" r="A7"/>
-      <c t="s" r="B7">
-        <v>12</v>
-      </c>
-      <c t="s" r="C7">
-        <v>16</v>
-      </c>
-      <c t="s" r="D7">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>